<commit_message>
updated cosmosdb to include serverless option
</commit_message>
<xml_diff>
--- a/Infrastructure LLD.xlsx
+++ b/Infrastructure LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ncea\ncea-infrastructure-core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C53276-0DB9-4278-9128-8EED632029E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8205338-FE90-42A1-A74E-A95BDE3220EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B9976C2E-3E3B-4988-8FAF-E5DC2F2CC586}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Pre-requisites</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Finalise naming convention</t>
+  </si>
+  <si>
+    <t>Is it possible to get a service endpoint created in the SANDBOX to create the end to end devops pipeline</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0523B-932A-45E4-A7FF-8B3D8E600AB1}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,94 +480,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -609,7 +606,7 @@
       <c r="A30" s="3"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -625,6 +622,9 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Redis and blob storage
</commit_message>
<xml_diff>
--- a/Infrastructure LLD.xlsx
+++ b/Infrastructure LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ncea\ncea-infrastructure-core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8205338-FE90-42A1-A74E-A95BDE3220EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D798704D-B027-4DCF-B3D2-4DCE27ADACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B9976C2E-3E3B-4988-8FAF-E5DC2F2CC586}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Pre-requisites</t>
   </si>
@@ -95,6 +95,57 @@
   </si>
   <si>
     <t>Is it possible to get a service endpoint created in the SANDBOX to create the end to end devops pipeline</t>
+  </si>
+  <si>
+    <t>Review available templates:
+https://dev.azure.com/defragovuk/DEFRA-DEVOPS-COMMON/_git/Defra.Infrastructure.Common?path=/templates/Microsoft.Network</t>
+  </si>
+  <si>
+    <t>Role assignments - how do we handle? I intend to use the rbac model.
+Ideally want to set all of these permissions in the pipeline, e.g webapp can get a secret from the keyvautl</t>
+  </si>
+  <si>
+    <t>Git hub actions or dev ops pipelines?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALI </t>
+  </si>
+  <si>
+    <t>Devop engineer</t>
+  </si>
+  <si>
+    <t>Jevgenijs</t>
+  </si>
+  <si>
+    <t>F5 silverline</t>
+  </si>
+  <si>
+    <t>Pieplines and current project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali to do </t>
+  </si>
+  <si>
+    <t>App registration and rbac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resources Will be connected to central LA.
+</t>
+  </si>
+  <si>
+    <t>Front end ingress point</t>
+  </si>
+  <si>
+    <t>All egress goes via palo alto.</t>
+  </si>
+  <si>
+    <t>TBD. CCOE engineer allocated to work through.</t>
+  </si>
+  <si>
+    <t>Next steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali to catch up and start </t>
   </si>
 </sst>
 </file>
@@ -455,24 +506,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0523B-932A-45E4-A7FF-8B3D8E600AB1}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -480,142 +532,187 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="3"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -625,6 +722,15 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the TODO list in LLD spreadsheet
</commit_message>
<xml_diff>
--- a/Infrastructure LLD.xlsx
+++ b/Infrastructure LLD.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ncea\ncea-infrastructure-core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D798704D-B027-4DCF-B3D2-4DCE27ADACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5356DA-30AE-42EB-B37A-4F459E493712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B9976C2E-3E3B-4988-8FAF-E5DC2F2CC586}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TODO" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>Pre-requisites</t>
   </si>
@@ -147,14 +148,166 @@
   <si>
     <t xml:space="preserve">Ali to catch up and start </t>
   </si>
+  <si>
+    <t>IAC to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>VNET to be added with two subnets:
+1. Private endpoints
+2. AppService subnet (delegated to 'Microsoft.Web/serverFarms'</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Route table with default routes to be added</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Assume access to platform URLS included in default firewall rules</t>
+  </si>
+  <si>
+    <t>RBAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automate assignment of 'Key Vault Secrets User' on the KeyVault for the following system assigned managed identities:
+1. Web App Front End
+2. Web App API
+3. Cosmos DB
+4. Data Factory
+</t>
+  </si>
+  <si>
+    <t>Permission ID:
+Key Vault Secrets User: 4633458b-17de-408a-b874-0445c86b69e6</t>
+  </si>
+  <si>
+    <t>Permission ID:
+Storage Blob Data Contributor: ba92f5b4-2d11-453d-a403-e96b0029c9fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automate assignment of 'Storage Blob Data Contributor' for managed identity:
+1. Data Factory
+</t>
+  </si>
+  <si>
+    <t>Automate assignment of 'Cosmos DB Built-in Data Contributor' for managed identity:
+1. Data factory
+2. Web App Api</t>
+  </si>
+  <si>
+    <t>Automate assignment of 'AcrPull' to managed identities:
+1. Web App Front End
+2. Web App API</t>
+  </si>
+  <si>
+    <t>Permission ID: 
+AcrPull: 7f951dda-4ed3-4680-a7ca-43fe172d538d</t>
+  </si>
+  <si>
+    <t>DevOps service principal added to DevOps project with permissions to deploy to dev azure sub 'AZR-NCE-DEV1' :
+https://dev.azure.com/defragovuk/DEFRA-NCEA/</t>
+  </si>
+  <si>
+    <t>DevOps service principal added to DevOps project with permissions to push to container registry 
+https://dev.azure.com/defragovuk/DEFRA-NCEA/</t>
+  </si>
+  <si>
+    <t>DevOps RBAC</t>
+  </si>
+  <si>
+    <t>Permission ID:
+AcrPush: 8311e382-0749-4cb8-b61a-304f252e45ec</t>
+  </si>
+  <si>
+    <t>Permission ID:
+CCOE to define</t>
+  </si>
+  <si>
+    <t>Web App Auth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web App  Front end to be enabled for 'Entra ID' authentication:
+App registration to:
+1. Require authentication
+2. Unauthenticated requests to HTTP 403 Forbidden
+3. Access to the web app to be allowed in app registration, select users
+</t>
+  </si>
+  <si>
+    <t>Web App API  to be enabled for 'Entra ID' authentication:
+App registration to:
+1. Require authentication
+2. Unauthorised to  HTTP 401
+This needs to be integrated with the API Management API. 
+To be defined.</t>
+  </si>
+  <si>
+    <t>API App Auth</t>
+  </si>
+  <si>
+    <t>Azure RBAC</t>
+  </si>
+  <si>
+    <t>Access to Azure Dev 'AZR-NCE-DEV1' to be able to manage and troubleshoot infra.
+Contributor?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automate adding all private endpoints to private dns zones.
+Ensure private dns zones are integrated with the VNET and are resolvable. </t>
+  </si>
+  <si>
+    <t>Permission ID:
+Cosmos DB Built-in Data Contributor: 00000000-0000-0000-0000-000000000002
+This is not a default build in role. (https://learn.microsoft.com/en-us/answers/questions/994687/missing-cosmos-db-built-in-data-reader-and-cosmos)
+Following az cli command will show the role details:
+'az cosmosdb sql role definition list --account-name nceapoc-snd-cosmosdb --resource-group NCE-IAC-POC'</t>
+  </si>
+  <si>
+    <t>Private endpoints and DNS</t>
+  </si>
+  <si>
+    <t>Automate backup schedule for CosmosDB.
+LRS for lower environments</t>
+  </si>
+  <si>
+    <t>Backup</t>
+  </si>
+  <si>
+    <t>Ingress connectivity to Web Front End.
+How to restrict? Assume IP restriction however team are not using Defra laptops.</t>
+  </si>
+  <si>
+    <t>Ingress API connectivity to APIM.
+How to restrict? Assume IP restriction however team are not using Defra laptops.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -181,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,6 +344,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,10 +667,254 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3005D11-5A39-4219-A1D8-044845E7A2E7}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0523B-932A-45E4-A7FF-8B3D8E600AB1}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>